<commit_message>
Opdracht 3 week 4 is af
</commit_message>
<xml_diff>
--- a/detailedRetail.xlsx
+++ b/detailedRetail.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\873446\Office 365 Fontys\TW - ds - ds5\Week 4\homework assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/46d9bc8e4b2e6b05/Bureaublad/Fontys/DS5/VS code spul/ds5_assignment_group5/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_C5067629AEE16AFB2E26950392AF7FF6C912DC90" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E0281F9-B47E-4375-983F-B3B0381CD344}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7884"/>
+    <workbookView xWindow="-28920" yWindow="-7005" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="2" r:id="rId1"/>
@@ -188,7 +189,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -221,7 +222,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -498,16 +499,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.33203125" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3050,6 +3052,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004A262539C92C904585DD8DAEB62D4B9C" ma:contentTypeVersion="12" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="5204a78b4d4a8ddcdc2c8dcd1900bb37">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f033d15c-9de3-4438-afcc-4066b3eaa3a4" xmlns:ns3="9698003e-3bd0-412e-8c03-32e4ece41802" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae51eb4cb76dc66cd21afc4fb3030b9f" ns2:_="" ns3:_="">
     <xsd:import namespace="f033d15c-9de3-4438-afcc-4066b3eaa3a4"/>
@@ -3258,22 +3275,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C324E9F8-E6A9-48E7-8006-BD0484ADC6CC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="f033d15c-9de3-4438-afcc-4066b3eaa3a4"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9698003e-3bd0-412e-8c03-32e4ece41802"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD83FB53-9E8C-4CCD-9AD9-795BC9AB81B7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD91B230-535A-4F31-93DE-2C24F12F62E6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3290,29 +3317,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD83FB53-9E8C-4CCD-9AD9-795BC9AB81B7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C324E9F8-E6A9-48E7-8006-BD0484ADC6CC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="f033d15c-9de3-4438-afcc-4066b3eaa3a4"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9698003e-3bd0-412e-8c03-32e4ece41802"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>